<commit_message>
'na 00h00' to x
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_KGO_2024.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_KGO_2024.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="147">
   <si>
     <t>03u00</t>
   </si>
@@ -63,9 +63,6 @@
     <t>23u05</t>
   </si>
   <si>
-    <t>9/03/24</t>
-  </si>
-  <si>
     <t>01u06</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
   </si>
   <si>
     <t>03u46</t>
-  </si>
-  <si>
-    <t>na 00u00</t>
   </si>
   <si>
     <t>12u30</t>
@@ -487,10 +481,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
-    <numFmt numFmtId="166" formatCode="dd\-mm\-yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -637,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -646,9 +639,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -679,9 +669,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -967,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -977,17 +964,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45352</v>
       </c>
@@ -998,7 +985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45353</v>
       </c>
@@ -1009,7 +996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45354</v>
       </c>
@@ -1020,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45355</v>
       </c>
@@ -1031,7 +1018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45356</v>
       </c>
@@ -1042,7 +1029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45357</v>
       </c>
@@ -1053,7 +1040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45358</v>
       </c>
@@ -1064,7 +1051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45359</v>
       </c>
@@ -1075,62 +1062,62 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>45360</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>45361</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>45362</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>45363</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>45364</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>45365</v>
       </c>
@@ -1141,7 +1128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>45366</v>
       </c>
@@ -1152,7 +1139,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>45367</v>
       </c>
@@ -1163,29 +1150,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>45368</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>45369</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>45370</v>
       </c>
@@ -1196,7 +1183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>45371</v>
       </c>
@@ -1207,128 +1194,128 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>45372</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>45373</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>45374</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>45375</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>45376</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>45377</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>45378</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>45379</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>45380</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>45381</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="11">
+        <v>45382</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="12">
-        <v>45382</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>45352</v>
       </c>
@@ -1339,7 +1326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>45353</v>
       </c>
@@ -1350,7 +1337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>45354</v>
       </c>
@@ -1361,7 +1348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>45355</v>
       </c>
@@ -1413,18 +1400,18 @@
         <v>8</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="10" t="s">
+      <c r="A41" s="1">
+        <v>45360</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -1432,10 +1419,10 @@
         <v>45361</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -1443,10 +1430,10 @@
         <v>45362</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -1454,10 +1441,10 @@
         <v>45363</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -1486,7 +1473,7 @@
       <c r="A47" s="1">
         <v>45366</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -1498,10 +1485,10 @@
         <v>45367</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1509,10 +1496,10 @@
         <v>45368</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1553,10 +1540,10 @@
         <v>45372</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1564,10 +1551,10 @@
         <v>45373</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1575,7 +1562,7 @@
         <v>45374</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>0</v>
@@ -1586,10 +1573,10 @@
         <v>45375</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -1597,10 +1584,10 @@
         <v>45376</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -1608,10 +1595,10 @@
         <v>45377</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -1619,10 +1606,10 @@
         <v>45378</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -1630,10 +1617,10 @@
         <v>45379</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -1641,10 +1628,10 @@
         <v>45380</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -1652,47 +1639,47 @@
         <v>45381</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="12">
+      <c r="A63" s="11">
         <v>45382</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="11">
+        <v>45383</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="11">
+        <v>45384</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C63" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="4">
-        <v>45383</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="4">
-        <v>45384</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C65" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="4">
+      <c r="A66" s="11">
         <v>45385</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -1703,139 +1690,139 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="4">
+      <c r="A67" s="11">
         <v>45386</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="4">
+      <c r="A68" s="11">
         <v>45387</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="4">
+      <c r="A69" s="11">
         <v>45388</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="4">
+      <c r="A70" s="11">
         <v>45389</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="4">
+      <c r="A71" s="11">
         <v>45390</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" s="11">
+        <v>45391</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="4">
-        <v>45391</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="C72" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="4">
+      <c r="A73" s="11">
         <v>45392</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="4">
+      <c r="A74" s="11">
         <v>45393</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="4">
+      <c r="A75" s="11">
         <v>45394</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="4">
+      <c r="A76" s="11">
         <v>45395</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C76" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" s="11">
+        <v>45396</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" s="4">
-        <v>45396</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="4">
+      <c r="A78" s="11">
         <v>45397</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="4">
+      <c r="A79" s="11">
         <v>45398</v>
       </c>
       <c r="B79" s="2" t="s">
@@ -1846,7 +1833,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" s="4">
+      <c r="A80" s="11">
         <v>45399</v>
       </c>
       <c r="B80" s="2" t="s">
@@ -1857,7 +1844,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="4">
+      <c r="A81" s="11">
         <v>45400</v>
       </c>
       <c r="B81" s="2" t="s">
@@ -1868,168 +1855,168 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="4">
+      <c r="A82" s="11">
         <v>45401</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="4">
+      <c r="A83" s="11">
         <v>45402</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C83" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="11">
+        <v>45403</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" s="11">
+        <v>45404</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="11">
+        <v>45405</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="11">
+        <v>45406</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="11">
+        <v>45407</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" s="11">
+        <v>45408</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" s="11">
+        <v>45409</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="4">
-        <v>45403</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="4">
-        <v>45404</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="4">
-        <v>45405</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="4">
-        <v>45406</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="4">
-        <v>45407</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="4">
-        <v>45408</v>
-      </c>
-      <c r="B89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="4">
-        <v>45409</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="4">
+      <c r="A91" s="11">
         <v>45410</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="4">
+      <c r="A92" s="11">
         <v>45411</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" s="11">
+        <v>45412</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="4">
-        <v>45412</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="15">
+      <c r="A94" s="11">
         <v>45413</v>
       </c>
-      <c r="B94" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C94" s="13" t="s">
+      <c r="B94" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C94" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="15">
+      <c r="A95" s="11">
         <v>45414</v>
       </c>
-      <c r="B95" s="13"/>
-      <c r="C95" s="13"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="12"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="4">
+      <c r="A96" s="11">
         <v>45383</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="4">
+      <c r="A97" s="11">
         <v>45384</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -2040,7 +2027,7 @@
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="4">
+      <c r="A98" s="11">
         <v>45385</v>
       </c>
       <c r="B98" s="2" t="s">
@@ -2051,51 +2038,51 @@
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="4">
+      <c r="A99" s="11">
         <v>45386</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" s="4">
+      <c r="A100" s="11">
         <v>45387</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" s="4">
+      <c r="A101" s="11">
         <v>45388</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="4">
+      <c r="A102" s="11">
         <v>45389</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="4">
+      <c r="A103" s="11">
         <v>45390</v>
       </c>
       <c r="B103" s="2" t="s">
@@ -2106,82 +2093,82 @@
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" s="4">
+      <c r="A104" s="11">
         <v>45391</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="4">
+      <c r="A105" s="11">
         <v>45392</v>
       </c>
       <c r="B105" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C105" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C105" s="3" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" s="4">
+      <c r="A106" s="11">
         <v>45393</v>
       </c>
       <c r="B106" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C106" s="3" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" s="4">
+      <c r="A107" s="11">
         <v>45394</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" s="4">
+      <c r="A108" s="11">
         <v>45395</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="4">
+      <c r="A109" s="11">
         <v>45396</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C109" s="3"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A110" s="4">
+      <c r="A110" s="11">
         <v>45397</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A111" s="4">
+      <c r="A111" s="11">
         <v>45398</v>
       </c>
       <c r="B111" s="2" t="s">
@@ -2192,18 +2179,18 @@
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A112" s="4">
+      <c r="A112" s="11">
         <v>45399</v>
       </c>
-      <c r="B112" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C112" s="9" t="s">
+      <c r="B112" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C112" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A113" s="4">
+      <c r="A113" s="11">
         <v>45400</v>
       </c>
       <c r="B113" s="2" t="s">
@@ -2214,62 +2201,62 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" s="4">
+      <c r="A114" s="11">
         <v>45401</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" s="4">
+      <c r="A115" s="11">
         <v>45402</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C115" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" s="11">
+        <v>45403</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" s="4">
-        <v>45403</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" s="4">
+      <c r="A117" s="11">
         <v>45404</v>
       </c>
       <c r="B117" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" s="11">
+        <v>45405</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C118" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C117" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A118" s="4">
-        <v>45405</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>126</v>
-      </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A119" s="4">
+      <c r="A119" s="11">
         <v>45406</v>
       </c>
       <c r="B119" s="2" t="s">
@@ -2280,51 +2267,51 @@
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A120" s="4">
+      <c r="A120" s="11">
         <v>45407</v>
       </c>
       <c r="B120" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" s="11">
+        <v>45408</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C120" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A121" s="4">
-        <v>45408</v>
-      </c>
-      <c r="B121" s="2" t="s">
+      <c r="C121" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C121" s="3" t="s">
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" s="11">
+        <v>45409</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A122" s="4">
-        <v>45409</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="C122" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" s="11">
+        <v>45410</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A123" s="4">
-        <v>45410</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="C123" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A124" s="4">
+      <c r="A124" s="11">
         <v>45411</v>
       </c>
       <c r="B124" s="2" t="s">
@@ -2335,29 +2322,29 @@
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A125" s="4">
+      <c r="A125" s="11">
         <v>45412</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A126" s="15">
+      <c r="A126" s="11">
         <v>45413</v>
       </c>
-      <c r="B126" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C126" s="14" t="s">
+      <c r="B126" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C126" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A127" s="15">
+      <c r="A127" s="11">
         <v>45414</v>
       </c>
     </row>

</xml_diff>